<commit_message>
Delete duplicates from airport and city dictionaries
</commit_message>
<xml_diff>
--- a/Data dict - airport_codes_and_city_id.xlsx
+++ b/Data dict - airport_codes_and_city_id.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwoom\Documents\Airline Reviews Data Cleaning\In Progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwoom\Documents\Airline Reviews Data Cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9804563-E2CB-4E9B-BF0D-679C759C0A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51413F3-D046-4173-A8A0-C57A46E4C329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{116977CA-72E9-471D-B0A1-D5D2AD6E37CC}"/>
   </bookViews>
@@ -12151,8 +12151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C42DFC-4223-4F7B-9B05-4C067574FB9B}">
   <dimension ref="A1:C3588"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A3566" zoomScale="93" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="C3566" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41511,7 +41511,7 @@
         <v>2960</v>
       </c>
       <c r="C3581">
-        <v>2883</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="3582" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add more missing airport codes and cities to dictionaries
</commit_message>
<xml_diff>
--- a/Data dict - airport_codes_and_city_id.xlsx
+++ b/Data dict - airport_codes_and_city_id.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwoom\Documents\Airline Reviews Data Cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51413F3-D046-4173-A8A0-C57A46E4C329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700647CA-5EA8-4BDC-84C9-FD6C56816EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{116977CA-72E9-471D-B0A1-D5D2AD6E37CC}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{116977CA-72E9-471D-B0A1-D5D2AD6E37CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3829" uniqueCount="3751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3843" uniqueCount="3765">
   <si>
     <t>ABR</t>
   </si>
@@ -11289,6 +11289,48 @@
   </si>
   <si>
     <t>Argyle International Airport</t>
+  </si>
+  <si>
+    <t>SHA</t>
+  </si>
+  <si>
+    <t>RAK</t>
+  </si>
+  <si>
+    <t>KNO</t>
+  </si>
+  <si>
+    <t>PGD</t>
+  </si>
+  <si>
+    <t>BLQ</t>
+  </si>
+  <si>
+    <t>AZA</t>
+  </si>
+  <si>
+    <t>KOE</t>
+  </si>
+  <si>
+    <t>Shanghai Hongqiao International Airport</t>
+  </si>
+  <si>
+    <t>Marrakesh Menara Airport</t>
+  </si>
+  <si>
+    <t>Kualanamu International Airport</t>
+  </si>
+  <si>
+    <t>Punta Gorda Airport</t>
+  </si>
+  <si>
+    <t>Bologna Guglielmo Marconi Airport</t>
+  </si>
+  <si>
+    <t>Phoenix-Mesa Gateway Airport</t>
+  </si>
+  <si>
+    <t>El Tari Airport</t>
   </si>
 </sst>
 </file>
@@ -12149,10 +12191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C42DFC-4223-4F7B-9B05-4C067574FB9B}">
-  <dimension ref="A1:C3588"/>
+  <dimension ref="A1:C3595"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3566" zoomScale="93" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C3566" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A3581" zoomScale="141" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D3585" sqref="D3585"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41585,6 +41627,83 @@
         <v>1348</v>
       </c>
     </row>
+    <row r="3589" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3589" t="s">
+        <v>3751</v>
+      </c>
+      <c r="B3589" t="s">
+        <v>3758</v>
+      </c>
+      <c r="C3589">
+        <v>2803</v>
+      </c>
+    </row>
+    <row r="3590" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3590" t="s">
+        <v>3752</v>
+      </c>
+      <c r="B3590" t="s">
+        <v>3759</v>
+      </c>
+      <c r="C3590">
+        <v>3445</v>
+      </c>
+    </row>
+    <row r="3591" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3591" t="s">
+        <v>3753</v>
+      </c>
+      <c r="B3591" t="s">
+        <v>3760</v>
+      </c>
+      <c r="C3591">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="3592" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3592" t="s">
+        <v>3754</v>
+      </c>
+      <c r="B3592" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C3592">
+        <v>3484</v>
+      </c>
+    </row>
+    <row r="3593" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3593" t="s">
+        <v>3755</v>
+      </c>
+      <c r="B3593" t="s">
+        <v>3762</v>
+      </c>
+      <c r="C3593">
+        <v>3485</v>
+      </c>
+    </row>
+    <row r="3594" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3594" t="s">
+        <v>3756</v>
+      </c>
+      <c r="B3594" t="s">
+        <v>3763</v>
+      </c>
+      <c r="C3594">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="3595" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3595" t="s">
+        <v>3757</v>
+      </c>
+      <c r="B3595" t="s">
+        <v>3764</v>
+      </c>
+      <c r="C3595">
+        <v>3487</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C3589" xr:uid="{B6C42DFC-4223-4F7B-9B05-4C067574FB9B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update city and airport dictionaries
By adding cities and airport information and correcting some entries.
</commit_message>
<xml_diff>
--- a/Data dict - airport_codes_and_city_id.xlsx
+++ b/Data dict - airport_codes_and_city_id.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwoom\Documents\Airline Reviews Data Cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700647CA-5EA8-4BDC-84C9-FD6C56816EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E4937F-8A9E-461E-A367-AB8B866C528D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{116977CA-72E9-471D-B0A1-D5D2AD6E37CC}"/>
+    <workbookView xWindow="11520" yWindow="576" windowWidth="10212" windowHeight="7968" xr2:uid="{116977CA-72E9-471D-B0A1-D5D2AD6E37CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3843" uniqueCount="3765">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3847" uniqueCount="3769">
   <si>
     <t>ABR</t>
   </si>
@@ -11102,12 +11102,6 @@
     <t>Mehrabad</t>
   </si>
   <si>
-    <t>Norte Los Rodeos</t>
-  </si>
-  <si>
-    <t>Sur Reina Sofia</t>
-  </si>
-  <si>
     <t>Haneda</t>
   </si>
   <si>
@@ -11331,6 +11325,24 @@
   </si>
   <si>
     <t>El Tari Airport</t>
+  </si>
+  <si>
+    <t>Shanghai Pudong International Airport</t>
+  </si>
+  <si>
+    <t>Kefalonia International Airport</t>
+  </si>
+  <si>
+    <t>East Midlands Airport</t>
+  </si>
+  <si>
+    <t>Santiago International Airport</t>
+  </si>
+  <si>
+    <t>Tenerife South Airport</t>
+  </si>
+  <si>
+    <t>Tenerife North–Ciudad de La Laguna Airport</t>
   </si>
 </sst>
 </file>
@@ -12193,8 +12205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C42DFC-4223-4F7B-9B05-4C067574FB9B}">
   <dimension ref="A1:C3595"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3581" zoomScale="141" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D3585" sqref="D3585"/>
+    <sheetView tabSelected="1" topLeftCell="A3130" zoomScale="141" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B3133" sqref="B3133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12205,13 +12217,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3698</v>
+        <v>3696</v>
       </c>
       <c r="B1" t="s">
-        <v>3702</v>
+        <v>3700</v>
       </c>
       <c r="C1" t="s">
-        <v>3749</v>
+        <v>3747</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -12838,7 +12850,7 @@
         <v>1085</v>
       </c>
       <c r="B79" t="s">
-        <v>3725</v>
+        <v>3723</v>
       </c>
       <c r="C79">
         <v>76</v>
@@ -13680,10 +13692,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>3710</v>
+        <v>3708</v>
       </c>
       <c r="B182" t="s">
-        <v>3720</v>
+        <v>3718</v>
       </c>
       <c r="C182">
         <v>3469</v>
@@ -14281,7 +14293,7 @@
         <v>1226</v>
       </c>
       <c r="B256" t="s">
-        <v>3734</v>
+        <v>3732</v>
       </c>
       <c r="C256">
         <v>250</v>
@@ -15732,7 +15744,7 @@
         <v>71</v>
       </c>
       <c r="B434" t="s">
-        <v>3726</v>
+        <v>3724</v>
       </c>
       <c r="C434">
         <v>419</v>
@@ -18895,10 +18907,10 @@
     </row>
     <row r="820" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A820" t="s">
-        <v>3736</v>
+        <v>3734</v>
       </c>
       <c r="B820" t="s">
-        <v>3737</v>
+        <v>3735</v>
       </c>
       <c r="C820">
         <v>751</v>
@@ -22145,7 +22157,7 @@
         <v>790</v>
       </c>
       <c r="B1218" t="s">
-        <v>3727</v>
+        <v>3725</v>
       </c>
       <c r="C1218">
         <v>1169</v>
@@ -22536,7 +22548,7 @@
         <v>1898</v>
       </c>
       <c r="B1265" t="s">
-        <v>3700</v>
+        <v>3698</v>
       </c>
       <c r="C1265">
         <v>1215</v>
@@ -22954,7 +22966,7 @@
         <v>277</v>
       </c>
       <c r="B1315" t="s">
-        <v>3701</v>
+        <v>3699</v>
       </c>
       <c r="C1315">
         <v>1264</v>
@@ -23951,7 +23963,7 @@
         <v>2011</v>
       </c>
       <c r="B1437" t="s">
-        <v>3748</v>
+        <v>3746</v>
       </c>
       <c r="C1437">
         <v>1384</v>
@@ -24824,6 +24836,9 @@
       <c r="A1544" t="s">
         <v>2086</v>
       </c>
+      <c r="B1544" t="s">
+        <v>3764</v>
+      </c>
       <c r="C1544">
         <v>1491</v>
       </c>
@@ -25055,7 +25070,7 @@
         <v>2959</v>
       </c>
       <c r="B1572" t="s">
-        <v>3743</v>
+        <v>3741</v>
       </c>
       <c r="C1572">
         <v>2686</v>
@@ -25918,7 +25933,7 @@
         <v>319</v>
       </c>
       <c r="B1678" t="s">
-        <v>3744</v>
+        <v>3742</v>
       </c>
       <c r="C1678">
         <v>1690</v>
@@ -26292,7 +26307,7 @@
         <v>2168</v>
       </c>
       <c r="B1724" t="s">
-        <v>3745</v>
+        <v>3743</v>
       </c>
       <c r="C1724">
         <v>1701</v>
@@ -27525,7 +27540,7 @@
         <v>2325</v>
       </c>
       <c r="B1874" t="s">
-        <v>3724</v>
+        <v>3722</v>
       </c>
       <c r="C1874">
         <v>1811</v>
@@ -28848,7 +28863,7 @@
         <v>307</v>
       </c>
       <c r="B2036" t="s">
-        <v>3746</v>
+        <v>3744</v>
       </c>
       <c r="C2036">
         <v>1887</v>
@@ -29654,7 +29669,7 @@
         <v>2521</v>
       </c>
       <c r="B2133" t="s">
-        <v>3723</v>
+        <v>3721</v>
       </c>
       <c r="C2133">
         <v>2054</v>
@@ -30542,7 +30557,7 @@
         <v>438</v>
       </c>
       <c r="B2241" t="s">
-        <v>3730</v>
+        <v>3728</v>
       </c>
       <c r="C2241">
         <v>2156</v>
@@ -30998,6 +31013,9 @@
       <c r="A2297" t="s">
         <v>2631</v>
       </c>
+      <c r="B2297" t="s">
+        <v>3765</v>
+      </c>
       <c r="C2297">
         <v>2211</v>
       </c>
@@ -31494,7 +31512,7 @@
         <v>463</v>
       </c>
       <c r="B2357" t="s">
-        <v>3731</v>
+        <v>3729</v>
       </c>
       <c r="C2357">
         <v>2269</v>
@@ -32605,10 +32623,10 @@
     </row>
     <row r="2491" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2491" t="s">
-        <v>3738</v>
+        <v>3736</v>
       </c>
       <c r="B2491" t="s">
-        <v>3739</v>
+        <v>3737</v>
       </c>
       <c r="C2491">
         <v>2269</v>
@@ -35641,6 +35659,9 @@
       <c r="A2862" t="s">
         <v>3004</v>
       </c>
+      <c r="B2862" t="s">
+        <v>3766</v>
+      </c>
       <c r="C2862">
         <v>2750</v>
       </c>
@@ -36162,6 +36183,9 @@
       <c r="A2923" t="s">
         <v>3042</v>
       </c>
+      <c r="B2923" t="s">
+        <v>3763</v>
+      </c>
       <c r="C2923">
         <v>2803</v>
       </c>
@@ -36679,7 +36703,7 @@
         <v>439</v>
       </c>
       <c r="B2986" t="s">
-        <v>3735</v>
+        <v>3733</v>
       </c>
       <c r="C2986">
         <v>2157</v>
@@ -36829,7 +36853,7 @@
         <v>3088</v>
       </c>
       <c r="B3004" t="s">
-        <v>3750</v>
+        <v>3748</v>
       </c>
       <c r="C3004">
         <v>3471</v>
@@ -36952,7 +36976,7 @@
         <v>482</v>
       </c>
       <c r="B3019" t="s">
-        <v>3747</v>
+        <v>3745</v>
       </c>
       <c r="C3019">
         <v>2387</v>
@@ -36971,7 +36995,7 @@
         <v>482</v>
       </c>
       <c r="B3021" t="s">
-        <v>3747</v>
+        <v>3745</v>
       </c>
       <c r="C3021">
         <v>3098</v>
@@ -37410,7 +37434,7 @@
         <v>3137</v>
       </c>
       <c r="B3074" t="s">
-        <v>3732</v>
+        <v>3730</v>
       </c>
       <c r="C3074">
         <v>2943</v>
@@ -37891,7 +37915,7 @@
         <v>3183</v>
       </c>
       <c r="B3133" t="s">
-        <v>3688</v>
+        <v>3768</v>
       </c>
       <c r="C3133">
         <v>3001</v>
@@ -37902,7 +37926,7 @@
         <v>3184</v>
       </c>
       <c r="B3134" t="s">
-        <v>3689</v>
+        <v>3767</v>
       </c>
       <c r="C3134">
         <v>3002</v>
@@ -38409,7 +38433,7 @@
         <v>3230</v>
       </c>
       <c r="B3197" t="s">
-        <v>3690</v>
+        <v>3688</v>
       </c>
       <c r="C3197">
         <v>3064</v>
@@ -38420,7 +38444,7 @@
         <v>3231</v>
       </c>
       <c r="B3198" t="s">
-        <v>3691</v>
+        <v>3689</v>
       </c>
       <c r="C3198">
         <v>3064</v>
@@ -38549,7 +38573,7 @@
         <v>991</v>
       </c>
       <c r="B3213" t="s">
-        <v>3699</v>
+        <v>3697</v>
       </c>
       <c r="C3213">
         <v>3076</v>
@@ -38560,7 +38584,7 @@
         <v>992</v>
       </c>
       <c r="B3214" t="s">
-        <v>3733</v>
+        <v>3731</v>
       </c>
       <c r="C3214">
         <v>3076</v>
@@ -38955,7 +38979,7 @@
         <v>1133</v>
       </c>
       <c r="B3263" t="s">
-        <v>3742</v>
+        <v>3740</v>
       </c>
       <c r="C3263">
         <v>3473</v>
@@ -39652,7 +39676,7 @@
         <v>3346</v>
       </c>
       <c r="B3349" t="s">
-        <v>3692</v>
+        <v>3690</v>
       </c>
       <c r="C3349">
         <v>3209</v>
@@ -39802,7 +39826,7 @@
         <v>3360</v>
       </c>
       <c r="B3367" t="s">
-        <v>3694</v>
+        <v>3692</v>
       </c>
       <c r="C3367">
         <v>3225</v>
@@ -39813,7 +39837,7 @@
         <v>3359</v>
       </c>
       <c r="B3368" t="s">
-        <v>3693</v>
+        <v>3691</v>
       </c>
       <c r="C3368">
         <v>3225</v>
@@ -39923,7 +39947,7 @@
         <v>3369</v>
       </c>
       <c r="B3381" t="s">
-        <v>3695</v>
+        <v>3693</v>
       </c>
       <c r="C3381">
         <v>3237</v>
@@ -40961,7 +40985,7 @@
         <v>3447</v>
       </c>
       <c r="B3510" t="s">
-        <v>3696</v>
+        <v>3694</v>
       </c>
       <c r="C3510">
         <v>3362</v>
@@ -41372,7 +41396,7 @@
         <v>3489</v>
       </c>
       <c r="B3561" t="s">
-        <v>3697</v>
+        <v>3695</v>
       </c>
       <c r="C3561">
         <v>3413</v>
@@ -41484,10 +41508,10 @@
     </row>
     <row r="3575" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3575" t="s">
-        <v>3703</v>
+        <v>3701</v>
       </c>
       <c r="B3575" t="s">
-        <v>3713</v>
+        <v>3711</v>
       </c>
       <c r="C3575">
         <v>250</v>
@@ -41495,10 +41519,10 @@
     </row>
     <row r="3576" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3576" t="s">
-        <v>3704</v>
+        <v>3702</v>
       </c>
       <c r="B3576" t="s">
-        <v>3714</v>
+        <v>3712</v>
       </c>
       <c r="C3576">
         <v>2992</v>
@@ -41506,10 +41530,10 @@
     </row>
     <row r="3577" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3577" t="s">
-        <v>3705</v>
+        <v>3703</v>
       </c>
       <c r="B3577" t="s">
-        <v>3715</v>
+        <v>3713</v>
       </c>
       <c r="C3577">
         <v>3466</v>
@@ -41517,10 +41541,10 @@
     </row>
     <row r="3578" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3578" t="s">
-        <v>3706</v>
+        <v>3704</v>
       </c>
       <c r="B3578" t="s">
-        <v>3716</v>
+        <v>3714</v>
       </c>
       <c r="C3578">
         <v>3462</v>
@@ -41528,10 +41552,10 @@
     </row>
     <row r="3579" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3579" t="s">
-        <v>3707</v>
+        <v>3705</v>
       </c>
       <c r="B3579" t="s">
-        <v>3717</v>
+        <v>3715</v>
       </c>
       <c r="C3579">
         <v>1370</v>
@@ -41539,10 +41563,10 @@
     </row>
     <row r="3580" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3580" t="s">
-        <v>3708</v>
+        <v>3706</v>
       </c>
       <c r="B3580" t="s">
-        <v>3718</v>
+        <v>3716</v>
       </c>
       <c r="C3580">
         <v>3467</v>
@@ -41558,10 +41582,10 @@
     </row>
     <row r="3582" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3582" t="s">
-        <v>3709</v>
+        <v>3707</v>
       </c>
       <c r="B3582" t="s">
-        <v>3719</v>
+        <v>3717</v>
       </c>
       <c r="C3582">
         <v>3468</v>
@@ -41577,10 +41601,10 @@
     </row>
     <row r="3584" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3584" t="s">
-        <v>3712</v>
+        <v>3710</v>
       </c>
       <c r="B3584" t="s">
-        <v>3722</v>
+        <v>3720</v>
       </c>
       <c r="C3584">
         <v>82</v>
@@ -41588,10 +41612,10 @@
     </row>
     <row r="3585" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3585" t="s">
-        <v>3728</v>
+        <v>3726</v>
       </c>
       <c r="B3585" t="s">
-        <v>3729</v>
+        <v>3727</v>
       </c>
       <c r="C3585">
         <v>3470</v>
@@ -41599,10 +41623,10 @@
     </row>
     <row r="3586" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3586" t="s">
-        <v>3711</v>
+        <v>3709</v>
       </c>
       <c r="B3586" t="s">
-        <v>3721</v>
+        <v>3719</v>
       </c>
       <c r="C3586">
         <v>3474</v>
@@ -41618,10 +41642,10 @@
     </row>
     <row r="3588" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3588" t="s">
-        <v>3740</v>
+        <v>3738</v>
       </c>
       <c r="B3588" t="s">
-        <v>3741</v>
+        <v>3739</v>
       </c>
       <c r="C3588">
         <v>1348</v>
@@ -41629,10 +41653,10 @@
     </row>
     <row r="3589" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3589" t="s">
-        <v>3751</v>
+        <v>3749</v>
       </c>
       <c r="B3589" t="s">
-        <v>3758</v>
+        <v>3756</v>
       </c>
       <c r="C3589">
         <v>2803</v>
@@ -41640,10 +41664,10 @@
     </row>
     <row r="3590" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3590" t="s">
-        <v>3752</v>
+        <v>3750</v>
       </c>
       <c r="B3590" t="s">
-        <v>3759</v>
+        <v>3757</v>
       </c>
       <c r="C3590">
         <v>3445</v>
@@ -41651,10 +41675,10 @@
     </row>
     <row r="3591" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3591" t="s">
-        <v>3753</v>
+        <v>3751</v>
       </c>
       <c r="B3591" t="s">
-        <v>3760</v>
+        <v>3758</v>
       </c>
       <c r="C3591">
         <v>1904</v>
@@ -41662,10 +41686,10 @@
     </row>
     <row r="3592" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3592" t="s">
-        <v>3754</v>
+        <v>3752</v>
       </c>
       <c r="B3592" t="s">
-        <v>3761</v>
+        <v>3759</v>
       </c>
       <c r="C3592">
         <v>3484</v>
@@ -41673,10 +41697,10 @@
     </row>
     <row r="3593" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3593" t="s">
-        <v>3755</v>
+        <v>3753</v>
       </c>
       <c r="B3593" t="s">
-        <v>3762</v>
+        <v>3760</v>
       </c>
       <c r="C3593">
         <v>3485</v>
@@ -41684,10 +41708,10 @@
     </row>
     <row r="3594" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3594" t="s">
-        <v>3756</v>
+        <v>3754</v>
       </c>
       <c r="B3594" t="s">
-        <v>3763</v>
+        <v>3761</v>
       </c>
       <c r="C3594">
         <v>3486</v>
@@ -41695,10 +41719,10 @@
     </row>
     <row r="3595" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3595" t="s">
-        <v>3757</v>
+        <v>3755</v>
       </c>
       <c r="B3595" t="s">
-        <v>3764</v>
+        <v>3762</v>
       </c>
       <c r="C3595">
         <v>3487</v>

</xml_diff>